<commit_message>
Got new Pay Rate.xlsx
</commit_message>
<xml_diff>
--- a/Pay Rate.xlsx
+++ b/Pay Rate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McMullin Family\Desktop\Payroll-GH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3458B456-1478-4926-8C0C-118BD9133D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337526ED-6FAF-47E3-A595-5BB589320580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{C8A3C214-2E77-429D-96EA-CDDC55A45220}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Night Rate</t>
   </si>
@@ -62,12 +62,6 @@
     <t>KARI</t>
   </si>
   <si>
-    <t>DRIGGS</t>
-  </si>
-  <si>
-    <t>KAT</t>
-  </si>
-  <si>
     <t>ENAGBONRO</t>
   </si>
   <si>
@@ -143,12 +137,6 @@
     <t>FANNY</t>
   </si>
   <si>
-    <t>SILVA</t>
-  </si>
-  <si>
-    <t>SKYLEIGH</t>
-  </si>
-  <si>
     <t>VAITAI</t>
   </si>
   <si>
@@ -174,6 +162,12 @@
   </si>
   <si>
     <t>LILI</t>
+  </si>
+  <si>
+    <t>SARA</t>
+  </si>
+  <si>
+    <t>BERTEAUX</t>
   </si>
 </sst>
 </file>
@@ -655,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7BA016-8B11-48C7-9F82-F364EB8D8B29}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,10 +663,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -697,10 +691,10 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6">
         <v>18</v>
@@ -711,13 +705,13 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6">
         <v>16</v>
@@ -725,13 +719,13 @@
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="6">
         <v>16</v>
@@ -739,10 +733,10 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6">
         <v>17</v>
@@ -753,10 +747,10 @@
     </row>
     <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6">
         <v>22</v>
@@ -765,26 +759,26 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="6">
-        <v>18</v>
-      </c>
-      <c r="D8" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="6">
         <v>17</v>
@@ -795,10 +789,10 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6">
         <v>18</v>
@@ -809,10 +803,10 @@
     </row>
     <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
         <v>20</v>
@@ -823,10 +817,10 @@
     </row>
     <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <v>18</v>
@@ -837,10 +831,10 @@
     </row>
     <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
         <v>18</v>
@@ -851,10 +845,10 @@
     </row>
     <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6">
         <v>18</v>
@@ -865,38 +859,38 @@
     </row>
     <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="6">
-        <v>18</v>
-      </c>
-      <c r="D15" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="C16" s="9">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6">
-        <v>18</v>
-      </c>
-      <c r="D16" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="B17" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="9">
         <v>18</v>
@@ -907,10 +901,10 @@
     </row>
     <row r="18" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="9">
         <v>22</v>
@@ -921,13 +915,13 @@
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C19" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="9">
         <v>16</v>
@@ -935,10 +929,10 @@
     </row>
     <row r="20" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="9">
         <v>19</v>
@@ -949,34 +943,23 @@
     </row>
     <row r="21" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C21" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="9">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9">
-        <v>17</v>
-      </c>
-      <c r="D22" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D21">
+    <sortCondition ref="A3:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>